<commit_message>
Add the models to the output and the data to the excel of each instance
</commit_message>
<xml_diff>
--- a/outputs/Lib_1.xlsx
+++ b/outputs/Lib_1.xlsx
@@ -595,10 +595,10 @@
         <v>2014</v>
       </c>
       <c r="E2">
-        <v>4.547473508864641E-13</v>
+        <v>0</v>
       </c>
       <c r="F2">
-        <v>1195</v>
+        <v>661</v>
       </c>
     </row>
     <row r="3" spans="1:6">
@@ -618,7 +618,7 @@
         <v>0</v>
       </c>
       <c r="F3">
-        <v>3272</v>
+        <v>563</v>
       </c>
     </row>
     <row r="4" spans="1:6">
@@ -638,7 +638,7 @@
         <v>0</v>
       </c>
       <c r="F4">
-        <v>1148</v>
+        <v>614</v>
       </c>
     </row>
     <row r="5" spans="1:6">
@@ -652,13 +652,13 @@
         <v>7168</v>
       </c>
       <c r="D5">
-        <v>7167.999999999998</v>
+        <v>7168.000000000001</v>
       </c>
       <c r="E5">
-        <v>1.818989403545856E-12</v>
+        <v>9.094947017729282E-13</v>
       </c>
       <c r="F5">
-        <v>1856</v>
+        <v>1624</v>
       </c>
     </row>
     <row r="6" spans="1:6">
@@ -678,7 +678,7 @@
         <v>0</v>
       </c>
       <c r="F6">
-        <v>1722</v>
+        <v>1223</v>
       </c>
     </row>
     <row r="7" spans="1:6">
@@ -698,7 +698,7 @@
         <v>0</v>
       </c>
       <c r="F7">
-        <v>1890</v>
+        <v>1935</v>
       </c>
     </row>
     <row r="8" spans="1:6">
@@ -712,13 +712,13 @@
         <v>4366</v>
       </c>
       <c r="D8">
-        <v>4527</v>
+        <v>4365.999999999998</v>
       </c>
       <c r="E8">
-        <v>161</v>
+        <v>1.818989403545856E-12</v>
       </c>
       <c r="F8">
-        <v>4231</v>
+        <v>4567</v>
       </c>
     </row>
     <row r="9" spans="1:6">
@@ -732,13 +732,13 @@
         <v>7926</v>
       </c>
       <c r="D9">
-        <v>8282</v>
+        <v>7926</v>
       </c>
       <c r="E9">
-        <v>356</v>
+        <v>0</v>
       </c>
       <c r="F9">
-        <v>5009</v>
+        <v>12981</v>
       </c>
     </row>
     <row r="10" spans="1:6">
@@ -758,7 +758,7 @@
         <v>0</v>
       </c>
       <c r="F10">
-        <v>2779</v>
+        <v>2880</v>
       </c>
     </row>
     <row r="11" spans="1:6">
@@ -775,10 +775,10 @@
         <v>23112</v>
       </c>
       <c r="E11">
-        <v>3.637978807091713E-12</v>
+        <v>0</v>
       </c>
       <c r="F11">
-        <v>2946</v>
+        <v>2674</v>
       </c>
     </row>
     <row r="12" spans="1:6">
@@ -792,13 +792,13 @@
         <v>3447</v>
       </c>
       <c r="D12">
-        <v>3471.000000000002</v>
+        <v>3447</v>
       </c>
       <c r="E12">
-        <v>24.00000000000182</v>
+        <v>4.547473508864641E-13</v>
       </c>
       <c r="F12">
-        <v>4224</v>
+        <v>8166</v>
       </c>
     </row>
     <row r="13" spans="1:6">
@@ -818,7 +818,7 @@
         <v>0</v>
       </c>
       <c r="F13">
-        <v>4668</v>
+        <v>3923</v>
       </c>
     </row>
     <row r="14" spans="1:6">
@@ -832,13 +832,13 @@
         <v>3760</v>
       </c>
       <c r="D14">
-        <v>3779</v>
+        <v>3760</v>
       </c>
       <c r="E14">
-        <v>19.00000000000045</v>
+        <v>0</v>
       </c>
       <c r="F14">
-        <v>4299</v>
+        <v>5285</v>
       </c>
     </row>
     <row r="15" spans="1:6">
@@ -852,13 +852,13 @@
         <v>5965</v>
       </c>
       <c r="D15">
-        <v>5964.999999999989</v>
+        <v>5965</v>
       </c>
       <c r="E15">
-        <v>1.091393642127514E-11</v>
+        <v>0</v>
       </c>
       <c r="F15">
-        <v>4980</v>
+        <v>5831</v>
       </c>
     </row>
     <row r="16" spans="1:6">
@@ -872,13 +872,13 @@
         <v>7816</v>
       </c>
       <c r="D16">
-        <v>7816.000000000001</v>
+        <v>7816</v>
       </c>
       <c r="E16">
-        <v>9.094947017729282E-13</v>
+        <v>0</v>
       </c>
       <c r="F16">
-        <v>3982</v>
+        <v>5598</v>
       </c>
     </row>
     <row r="17" spans="1:6">
@@ -892,13 +892,13 @@
         <v>11543</v>
       </c>
       <c r="D17">
-        <v>11559</v>
+        <v>11543</v>
       </c>
       <c r="E17">
-        <v>16</v>
+        <v>0</v>
       </c>
       <c r="F17">
-        <v>4996</v>
+        <v>6643</v>
       </c>
     </row>
     <row r="18" spans="1:6">
@@ -912,13 +912,13 @@
         <v>9884</v>
       </c>
       <c r="D18">
-        <v>9935</v>
+        <v>9884</v>
       </c>
       <c r="E18">
-        <v>51</v>
+        <v>0</v>
       </c>
       <c r="F18">
-        <v>4984</v>
+        <v>8780</v>
       </c>
     </row>
     <row r="19" spans="1:6">
@@ -932,13 +932,13 @@
         <v>15607</v>
       </c>
       <c r="D19">
-        <v>16816</v>
+        <v>15607</v>
       </c>
       <c r="E19">
-        <v>1209</v>
+        <v>0</v>
       </c>
       <c r="F19">
-        <v>4988</v>
+        <v>10875</v>
       </c>
     </row>
     <row r="20" spans="1:6">
@@ -958,7 +958,7 @@
         <v>0</v>
       </c>
       <c r="F20">
-        <v>4063</v>
+        <v>11116</v>
       </c>
     </row>
     <row r="21" spans="1:6">
@@ -972,13 +972,13 @@
         <v>26561</v>
       </c>
       <c r="D21">
-        <v>27774</v>
+        <v>26561.00000000001</v>
       </c>
       <c r="E21">
-        <v>1213</v>
+        <v>7.275957614183426E-12</v>
       </c>
       <c r="F21">
-        <v>4900</v>
+        <v>72196</v>
       </c>
     </row>
     <row r="22" spans="1:6">
@@ -992,13 +992,13 @@
         <v>7295</v>
       </c>
       <c r="D22">
-        <v>7406</v>
+        <v>7295</v>
       </c>
       <c r="E22">
-        <v>111</v>
+        <v>0</v>
       </c>
       <c r="F22">
-        <v>4988</v>
+        <v>40366</v>
       </c>
     </row>
     <row r="23" spans="1:6">
@@ -1012,13 +1012,13 @@
         <v>3271</v>
       </c>
       <c r="D23">
-        <v>3279</v>
+        <v>3271</v>
       </c>
       <c r="E23">
-        <v>8</v>
+        <v>0</v>
       </c>
       <c r="F23">
-        <v>4993</v>
+        <v>5419</v>
       </c>
     </row>
     <row r="24" spans="1:6">
@@ -1032,13 +1032,13 @@
         <v>6036</v>
       </c>
       <c r="D24">
-        <v>6036.000000000002</v>
+        <v>6036</v>
       </c>
       <c r="E24">
-        <v>1.818989403545856E-12</v>
+        <v>0</v>
       </c>
       <c r="F24">
-        <v>2740</v>
+        <v>3418</v>
       </c>
     </row>
     <row r="25" spans="1:6">
@@ -1052,13 +1052,13 @@
         <v>6327</v>
       </c>
       <c r="D25">
-        <v>6390</v>
+        <v>6327</v>
       </c>
       <c r="E25">
-        <v>63</v>
+        <v>0</v>
       </c>
       <c r="F25">
-        <v>4225</v>
+        <v>4441</v>
       </c>
     </row>
     <row r="26" spans="1:6">
@@ -1078,7 +1078,7 @@
         <v>0</v>
       </c>
       <c r="F26">
-        <v>3103</v>
+        <v>2162</v>
       </c>
     </row>
     <row r="27" spans="1:6">
@@ -1092,13 +1092,13 @@
         <v>4448</v>
       </c>
       <c r="D27">
-        <v>4464</v>
+        <v>4448.000000000002</v>
       </c>
       <c r="E27">
-        <v>16</v>
+        <v>1.818989403545856E-12</v>
       </c>
       <c r="F27">
-        <v>4847</v>
+        <v>11238</v>
       </c>
     </row>
     <row r="28" spans="1:6">
@@ -1112,13 +1112,13 @@
         <v>10921</v>
       </c>
       <c r="D28">
-        <v>10977</v>
+        <v>10921</v>
       </c>
       <c r="E28">
-        <v>56</v>
+        <v>0</v>
       </c>
       <c r="F28">
-        <v>4995</v>
+        <v>7125</v>
       </c>
     </row>
     <row r="29" spans="1:6">
@@ -1132,13 +1132,13 @@
         <v>11117</v>
       </c>
       <c r="D29">
-        <v>11569</v>
+        <v>11117</v>
       </c>
       <c r="E29">
-        <v>452</v>
+        <v>0</v>
       </c>
       <c r="F29">
-        <v>4972</v>
+        <v>15268</v>
       </c>
     </row>
     <row r="30" spans="1:6">
@@ -1152,13 +1152,13 @@
         <v>9832</v>
       </c>
       <c r="D30">
-        <v>9850</v>
+        <v>9832</v>
       </c>
       <c r="E30">
-        <v>18</v>
+        <v>0</v>
       </c>
       <c r="F30">
-        <v>4978</v>
+        <v>14677</v>
       </c>
     </row>
     <row r="31" spans="1:6">
@@ -1172,13 +1172,13 @@
         <v>10816</v>
       </c>
       <c r="D31">
-        <v>11102</v>
+        <v>10816</v>
       </c>
       <c r="E31">
-        <v>286</v>
+        <v>0</v>
       </c>
       <c r="F31">
-        <v>4982</v>
+        <v>871670</v>
       </c>
     </row>
     <row r="32" spans="1:6">
@@ -1192,13 +1192,13 @@
         <v>4466</v>
       </c>
       <c r="D32">
-        <v>4563</v>
+        <v>4466</v>
       </c>
       <c r="E32">
-        <v>97</v>
+        <v>0</v>
       </c>
       <c r="F32">
-        <v>4980</v>
+        <v>17200</v>
       </c>
     </row>
     <row r="33" spans="1:6">
@@ -1212,13 +1212,13 @@
         <v>9881</v>
       </c>
       <c r="D33">
-        <v>9902</v>
+        <v>9880.999999999998</v>
       </c>
       <c r="E33">
-        <v>21</v>
+        <v>1.818989403545856E-12</v>
       </c>
       <c r="F33">
-        <v>4983</v>
+        <v>15855</v>
       </c>
     </row>
     <row r="34" spans="1:6">
@@ -1232,13 +1232,13 @@
         <v>39463</v>
       </c>
       <c r="D34">
-        <v>48963</v>
+        <v>39463</v>
       </c>
       <c r="E34">
-        <v>9500</v>
+        <v>0</v>
       </c>
       <c r="F34">
-        <v>4972</v>
+        <v>1199075</v>
       </c>
     </row>
     <row r="35" spans="1:6">
@@ -1252,13 +1252,13 @@
         <v>4701</v>
       </c>
       <c r="D35">
-        <v>4798</v>
+        <v>4701</v>
       </c>
       <c r="E35">
-        <v>97</v>
+        <v>0</v>
       </c>
       <c r="F35">
-        <v>4978</v>
+        <v>19753</v>
       </c>
     </row>
     <row r="36" spans="1:6">
@@ -1278,7 +1278,7 @@
         <v>0</v>
       </c>
       <c r="F36">
-        <v>2676</v>
+        <v>2086</v>
       </c>
     </row>
     <row r="37" spans="1:6">
@@ -1292,13 +1292,13 @@
         <v>16781</v>
       </c>
       <c r="D37">
-        <v>17244</v>
+        <v>16781</v>
       </c>
       <c r="E37">
-        <v>463</v>
+        <v>0</v>
       </c>
       <c r="F37">
-        <v>4280</v>
+        <v>36640</v>
       </c>
     </row>
     <row r="38" spans="1:6">
@@ -1312,13 +1312,13 @@
         <v>14668</v>
       </c>
       <c r="D38">
-        <v>14988</v>
+        <v>14668</v>
       </c>
       <c r="E38">
-        <v>320</v>
+        <v>0</v>
       </c>
       <c r="F38">
-        <v>4987</v>
+        <v>79614</v>
       </c>
     </row>
     <row r="39" spans="1:6">
@@ -1332,13 +1332,13 @@
         <v>47249</v>
       </c>
       <c r="D39">
-        <v>47289</v>
+        <v>47249</v>
       </c>
       <c r="E39">
-        <v>40</v>
+        <v>0</v>
       </c>
       <c r="F39">
-        <v>4971</v>
+        <v>20586</v>
       </c>
     </row>
     <row r="40" spans="1:6">
@@ -1352,13 +1352,13 @@
         <v>41007</v>
       </c>
       <c r="D40">
-        <v>43893</v>
+        <v>41007</v>
       </c>
       <c r="E40">
-        <v>2886</v>
+        <v>0</v>
       </c>
       <c r="F40">
-        <v>4980</v>
+        <v>88409</v>
       </c>
     </row>
     <row r="41" spans="1:6">
@@ -1372,13 +1372,13 @@
         <v>61633</v>
       </c>
       <c r="D41">
-        <v>65935</v>
+        <v>61636</v>
       </c>
       <c r="E41">
-        <v>4302</v>
+        <v>3</v>
       </c>
       <c r="F41">
-        <v>4979</v>
+        <v>1199401</v>
       </c>
     </row>
     <row r="42" spans="1:6">
@@ -1395,10 +1395,10 @@
         <v>17246</v>
       </c>
       <c r="E42">
-        <v>3.637978807091713E-12</v>
+        <v>0</v>
       </c>
       <c r="F42">
-        <v>3771</v>
+        <v>2998</v>
       </c>
     </row>
     <row r="43" spans="1:6">
@@ -1412,13 +1412,13 @@
         <v>7887</v>
       </c>
       <c r="D43">
-        <v>8344</v>
+        <v>7887</v>
       </c>
       <c r="E43">
-        <v>457</v>
+        <v>0</v>
       </c>
       <c r="F43">
-        <v>4176</v>
+        <v>10463</v>
       </c>
     </row>
     <row r="44" spans="1:6">
@@ -1432,13 +1432,13 @@
         <v>5114</v>
       </c>
       <c r="D44">
-        <v>5192</v>
+        <v>5114</v>
       </c>
       <c r="E44">
-        <v>78</v>
+        <v>0</v>
       </c>
       <c r="F44">
-        <v>4978</v>
+        <v>20970</v>
       </c>
     </row>
     <row r="45" spans="1:6">
@@ -1452,13 +1452,13 @@
         <v>36022</v>
       </c>
       <c r="D45">
-        <v>37329</v>
+        <v>37303</v>
       </c>
       <c r="E45">
-        <v>1307</v>
+        <v>1281</v>
       </c>
       <c r="F45">
-        <v>4989</v>
+        <v>1199242</v>
       </c>
     </row>
     <row r="46" spans="1:6">
@@ -1472,13 +1472,13 @@
         <v>17676</v>
       </c>
       <c r="D46">
-        <v>17819</v>
+        <v>17676</v>
       </c>
       <c r="E46">
-        <v>143</v>
+        <v>0</v>
       </c>
       <c r="F46">
-        <v>4938</v>
+        <v>4633</v>
       </c>
     </row>
     <row r="47" spans="1:6">
@@ -1492,13 +1492,13 @@
         <v>48701</v>
       </c>
       <c r="D47">
-        <v>51413</v>
+        <v>48701</v>
       </c>
       <c r="E47">
-        <v>2712</v>
+        <v>0</v>
       </c>
       <c r="F47">
-        <v>4977</v>
+        <v>177261</v>
       </c>
     </row>
     <row r="48" spans="1:6">
@@ -1512,13 +1512,13 @@
         <v>66230</v>
       </c>
       <c r="D48">
-        <v>69172</v>
+        <v>66230</v>
       </c>
       <c r="E48">
-        <v>2942</v>
+        <v>0</v>
       </c>
       <c r="F48">
-        <v>4966</v>
+        <v>659549</v>
       </c>
     </row>
     <row r="49" spans="1:6">
@@ -1532,13 +1532,13 @@
         <v>58964</v>
       </c>
       <c r="D49">
-        <v>60104.99999999999</v>
+        <v>58964</v>
       </c>
       <c r="E49">
-        <v>1140.999999999993</v>
+        <v>0</v>
       </c>
       <c r="F49">
-        <v>4967</v>
+        <v>65225</v>
       </c>
     </row>
     <row r="50" spans="1:6">
@@ -1552,13 +1552,13 @@
         <v>79614</v>
       </c>
       <c r="D50">
-        <v>85668</v>
+        <v>79659</v>
       </c>
       <c r="E50">
-        <v>6054</v>
+        <v>45</v>
       </c>
       <c r="F50">
-        <v>4966</v>
+        <v>1199777</v>
       </c>
     </row>
     <row r="51" spans="1:6">
@@ -1572,13 +1572,13 @@
         <v>5937</v>
       </c>
       <c r="D51">
-        <v>6032</v>
+        <v>5937</v>
       </c>
       <c r="E51">
-        <v>95</v>
+        <v>0</v>
       </c>
       <c r="F51">
-        <v>4976</v>
+        <v>29383</v>
       </c>
     </row>
     <row r="52" spans="1:6">
@@ -1592,13 +1592,13 @@
         <v>9060</v>
       </c>
       <c r="D52">
-        <v>9126</v>
+        <v>9060</v>
       </c>
       <c r="E52">
-        <v>66</v>
+        <v>0</v>
       </c>
       <c r="F52">
-        <v>4967</v>
+        <v>224940</v>
       </c>
     </row>
     <row r="53" spans="1:6">
@@ -1612,13 +1612,13 @@
         <v>34652</v>
       </c>
       <c r="D53">
-        <v>38575</v>
+        <v>34652</v>
       </c>
       <c r="E53">
-        <v>3923</v>
+        <v>0</v>
       </c>
       <c r="F53">
-        <v>4956</v>
+        <v>560694</v>
       </c>
     </row>
     <row r="54" spans="1:6">
@@ -1632,13 +1632,13 @@
         <v>30038</v>
       </c>
       <c r="D54">
-        <v>30458</v>
+        <v>30038</v>
       </c>
       <c r="E54">
-        <v>420</v>
+        <v>0</v>
       </c>
       <c r="F54">
-        <v>4967</v>
+        <v>33280</v>
       </c>
     </row>
     <row r="55" spans="1:6">
@@ -1652,13 +1652,13 @@
         <v>43853</v>
       </c>
       <c r="D55">
-        <v>51106</v>
+        <v>43853</v>
       </c>
       <c r="E55">
-        <v>7253</v>
+        <v>0</v>
       </c>
       <c r="F55">
-        <v>4972</v>
+        <v>10129</v>
       </c>
     </row>
     <row r="56" spans="1:6">
@@ -1672,13 +1672,13 @@
         <v>69610</v>
       </c>
       <c r="D56">
-        <v>70998</v>
+        <v>69753</v>
       </c>
       <c r="E56">
-        <v>1388</v>
+        <v>143</v>
       </c>
       <c r="F56">
-        <v>4949</v>
+        <v>1199989</v>
       </c>
     </row>
     <row r="57" spans="1:6">
@@ -1692,13 +1692,13 @@
         <v>64474</v>
       </c>
       <c r="D57">
-        <v>64474</v>
+        <v>64478</v>
       </c>
       <c r="E57">
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="F57">
-        <v>1193</v>
+        <v>1155</v>
       </c>
     </row>
     <row r="58" spans="1:6">
@@ -1718,7 +1718,7 @@
         <v>0</v>
       </c>
       <c r="F58">
-        <v>762</v>
+        <v>611</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Add outpul of Library 5_5
</commit_message>
<xml_diff>
--- a/outputs/Lib_1.xlsx
+++ b/outputs/Lib_1.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Universidade\2º Semestre\Simulação\SO_trabalho\outputs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9322FB33-CACA-4A40-8DF6-C4FFABC780B8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0E23BF76-C092-4241-8550-B114F00E96FF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="21820" windowHeight="13900" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -281,8 +281,9 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -624,12 +625,12 @@
   <dimension ref="A1:G58"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I9" sqref="I9:I10"/>
+      <selection activeCell="I14" sqref="I14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="6" max="6" width="11.81640625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="11.81640625" style="1" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:7" x14ac:dyDescent="0.35">
@@ -648,7 +649,7 @@
       <c r="E1" t="s">
         <v>70</v>
       </c>
-      <c r="F1" t="s">
+      <c r="F1" s="1" t="s">
         <v>4</v>
       </c>
       <c r="G1" t="s">
@@ -671,7 +672,7 @@
       <c r="E2">
         <v>0</v>
       </c>
-      <c r="F2">
+      <c r="F2" s="1">
         <f>(E2/C2)*100</f>
         <v>0</v>
       </c>
@@ -695,7 +696,7 @@
       <c r="E3">
         <v>0</v>
       </c>
-      <c r="F3">
+      <c r="F3" s="1">
         <f t="shared" ref="F3:F58" si="0">(E3/C3)*100</f>
         <v>0</v>
       </c>
@@ -719,7 +720,7 @@
       <c r="E4">
         <v>0</v>
       </c>
-      <c r="F4">
+      <c r="F4" s="1">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
@@ -743,7 +744,7 @@
       <c r="E5">
         <v>9.0949470177292824E-13</v>
       </c>
-      <c r="F5">
+      <c r="F5" s="1">
         <f t="shared" si="0"/>
         <v>1.2688263138573217E-14</v>
       </c>
@@ -767,7 +768,7 @@
       <c r="E6">
         <v>0</v>
       </c>
-      <c r="F6">
+      <c r="F6" s="1">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
@@ -791,7 +792,7 @@
       <c r="E7">
         <v>0</v>
       </c>
-      <c r="F7">
+      <c r="F7" s="1">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
@@ -815,7 +816,7 @@
       <c r="E8">
         <v>1.8189894035458561E-12</v>
       </c>
-      <c r="F8">
+      <c r="F8" s="1">
         <f t="shared" si="0"/>
         <v>4.1662606586025102E-14</v>
       </c>
@@ -839,7 +840,7 @@
       <c r="E9">
         <v>0</v>
       </c>
-      <c r="F9">
+      <c r="F9" s="1">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
@@ -863,7 +864,7 @@
       <c r="E10">
         <v>0</v>
       </c>
-      <c r="F10">
+      <c r="F10" s="1">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
@@ -887,7 +888,7 @@
       <c r="E11">
         <v>0</v>
       </c>
-      <c r="F11">
+      <c r="F11" s="1">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
@@ -911,7 +912,7 @@
       <c r="E12">
         <v>4.5474735088646412E-13</v>
       </c>
-      <c r="F12">
+      <c r="F12" s="1">
         <f t="shared" si="0"/>
         <v>1.3192554420843172E-14</v>
       </c>
@@ -935,7 +936,7 @@
       <c r="E13">
         <v>0</v>
       </c>
-      <c r="F13">
+      <c r="F13" s="1">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
@@ -959,7 +960,7 @@
       <c r="E14">
         <v>0</v>
       </c>
-      <c r="F14">
+      <c r="F14" s="1">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
@@ -983,7 +984,7 @@
       <c r="E15">
         <v>0</v>
       </c>
-      <c r="F15">
+      <c r="F15" s="1">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
@@ -1007,7 +1008,7 @@
       <c r="E16">
         <v>0</v>
       </c>
-      <c r="F16">
+      <c r="F16" s="1">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
@@ -1031,7 +1032,7 @@
       <c r="E17">
         <v>0</v>
       </c>
-      <c r="F17">
+      <c r="F17" s="1">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
@@ -1055,7 +1056,7 @@
       <c r="E18">
         <v>0</v>
       </c>
-      <c r="F18">
+      <c r="F18" s="1">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
@@ -1079,7 +1080,7 @@
       <c r="E19">
         <v>0</v>
       </c>
-      <c r="F19">
+      <c r="F19" s="1">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
@@ -1103,7 +1104,7 @@
       <c r="E20">
         <v>0</v>
       </c>
-      <c r="F20">
+      <c r="F20" s="1">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
@@ -1127,7 +1128,7 @@
       <c r="E21">
         <v>7.2759576141834259E-12</v>
       </c>
-      <c r="F21">
+      <c r="F21" s="1">
         <f t="shared" si="0"/>
         <v>2.739338735056446E-14</v>
       </c>
@@ -1151,7 +1152,7 @@
       <c r="E22">
         <v>0</v>
       </c>
-      <c r="F22">
+      <c r="F22" s="1">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
@@ -1175,7 +1176,7 @@
       <c r="E23">
         <v>0</v>
       </c>
-      <c r="F23">
+      <c r="F23" s="1">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
@@ -1199,7 +1200,7 @@
       <c r="E24">
         <v>0</v>
       </c>
-      <c r="F24">
+      <c r="F24" s="1">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
@@ -1223,7 +1224,7 @@
       <c r="E25">
         <v>0</v>
       </c>
-      <c r="F25">
+      <c r="F25" s="1">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
@@ -1247,7 +1248,7 @@
       <c r="E26">
         <v>0</v>
       </c>
-      <c r="F26">
+      <c r="F26" s="1">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
@@ -1271,7 +1272,7 @@
       <c r="E27">
         <v>1.8189894035458561E-12</v>
       </c>
-      <c r="F27">
+      <c r="F27" s="1">
         <f t="shared" si="0"/>
         <v>4.0894545943027341E-14</v>
       </c>
@@ -1295,7 +1296,7 @@
       <c r="E28">
         <v>0</v>
       </c>
-      <c r="F28">
+      <c r="F28" s="1">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
@@ -1319,7 +1320,7 @@
       <c r="E29">
         <v>0</v>
       </c>
-      <c r="F29">
+      <c r="F29" s="1">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
@@ -1343,7 +1344,7 @@
       <c r="E30">
         <v>0</v>
       </c>
-      <c r="F30">
+      <c r="F30" s="1">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
@@ -1367,7 +1368,7 @@
       <c r="E31">
         <v>0</v>
       </c>
-      <c r="F31">
+      <c r="F31" s="1">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
@@ -1391,7 +1392,7 @@
       <c r="E32">
         <v>0</v>
       </c>
-      <c r="F32">
+      <c r="F32" s="1">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
@@ -1415,7 +1416,7 @@
       <c r="E33">
         <v>1.8189894035458561E-12</v>
       </c>
-      <c r="F33">
+      <c r="F33" s="1">
         <f t="shared" si="0"/>
         <v>1.8408960667400628E-14</v>
       </c>
@@ -1439,7 +1440,7 @@
       <c r="E34">
         <v>0</v>
       </c>
-      <c r="F34">
+      <c r="F34" s="1">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
@@ -1463,7 +1464,7 @@
       <c r="E35">
         <v>0</v>
       </c>
-      <c r="F35">
+      <c r="F35" s="1">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
@@ -1487,7 +1488,7 @@
       <c r="E36">
         <v>0</v>
       </c>
-      <c r="F36">
+      <c r="F36" s="1">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
@@ -1511,7 +1512,7 @@
       <c r="E37">
         <v>0</v>
       </c>
-      <c r="F37">
+      <c r="F37" s="1">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
@@ -1535,7 +1536,7 @@
       <c r="E38">
         <v>0</v>
       </c>
-      <c r="F38">
+      <c r="F38" s="1">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
@@ -1559,7 +1560,7 @@
       <c r="E39">
         <v>0</v>
       </c>
-      <c r="F39">
+      <c r="F39" s="1">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
@@ -1583,7 +1584,7 @@
       <c r="E40">
         <v>0</v>
       </c>
-      <c r="F40">
+      <c r="F40" s="1">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
@@ -1607,7 +1608,7 @@
       <c r="E41">
         <v>3</v>
       </c>
-      <c r="F41">
+      <c r="F41" s="1">
         <f t="shared" si="0"/>
         <v>4.8675222689143803E-3</v>
       </c>
@@ -1631,7 +1632,7 @@
       <c r="E42">
         <v>0</v>
       </c>
-      <c r="F42">
+      <c r="F42" s="1">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
@@ -1655,7 +1656,7 @@
       <c r="E43">
         <v>0</v>
       </c>
-      <c r="F43">
+      <c r="F43" s="1">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
@@ -1679,7 +1680,7 @@
       <c r="E44">
         <v>0</v>
       </c>
-      <c r="F44">
+      <c r="F44" s="1">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
@@ -1703,7 +1704,7 @@
       <c r="E45">
         <v>1281</v>
       </c>
-      <c r="F45">
+      <c r="F45" s="1">
         <f t="shared" si="0"/>
         <v>3.556160124368442</v>
       </c>
@@ -1727,7 +1728,7 @@
       <c r="E46">
         <v>0</v>
       </c>
-      <c r="F46">
+      <c r="F46" s="1">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
@@ -1751,7 +1752,7 @@
       <c r="E47">
         <v>0</v>
       </c>
-      <c r="F47">
+      <c r="F47" s="1">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
@@ -1775,7 +1776,7 @@
       <c r="E48">
         <v>0</v>
       </c>
-      <c r="F48">
+      <c r="F48" s="1">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
@@ -1799,7 +1800,7 @@
       <c r="E49">
         <v>0</v>
       </c>
-      <c r="F49">
+      <c r="F49" s="1">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
@@ -1823,7 +1824,7 @@
       <c r="E50">
         <v>45</v>
       </c>
-      <c r="F50">
+      <c r="F50" s="1">
         <f t="shared" si="0"/>
         <v>5.6522722134297994E-2</v>
       </c>
@@ -1847,7 +1848,7 @@
       <c r="E51">
         <v>0</v>
       </c>
-      <c r="F51">
+      <c r="F51" s="1">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
@@ -1871,7 +1872,7 @@
       <c r="E52">
         <v>0</v>
       </c>
-      <c r="F52">
+      <c r="F52" s="1">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
@@ -1895,7 +1896,7 @@
       <c r="E53">
         <v>0</v>
       </c>
-      <c r="F53">
+      <c r="F53" s="1">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
@@ -1919,7 +1920,7 @@
       <c r="E54">
         <v>0</v>
       </c>
-      <c r="F54">
+      <c r="F54" s="1">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
@@ -1943,7 +1944,7 @@
       <c r="E55">
         <v>0</v>
       </c>
-      <c r="F55">
+      <c r="F55" s="1">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
@@ -1967,7 +1968,7 @@
       <c r="E56">
         <v>143</v>
       </c>
-      <c r="F56">
+      <c r="F56" s="1">
         <f t="shared" si="0"/>
         <v>0.20543025427381123</v>
       </c>
@@ -1991,7 +1992,7 @@
       <c r="E57">
         <v>4</v>
       </c>
-      <c r="F57">
+      <c r="F57" s="1">
         <f t="shared" si="0"/>
         <v>6.2040512454632872E-3</v>
       </c>
@@ -2015,7 +2016,7 @@
       <c r="E58">
         <v>0</v>
       </c>
-      <c r="F58">
+      <c r="F58" s="1">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>

</xml_diff>